<commit_message>
update cleanup with visualizations
</commit_message>
<xml_diff>
--- a/extraction consolidation results_V0_1.xlsx
+++ b/extraction consolidation results_V0_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac130903\Desktop\MDE4DT\mde4dts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7C7CEB3-AB6E-4759-8F51-B2365CC8DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E7A9595-4895-4044-8CE0-85B0DBDBBF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D11C759-8767-4256-9E25-90A34587B317}"/>
   </bookViews>
@@ -1102,21 +1102,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1243,30 +1234,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="4" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1780,8 +1771,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C290CE9-14EA-4DF4-9360-C084CCC50C1B}" name="Tabelle1" displayName="Tabelle1" ref="A1:T78" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:T78" xr:uid="{2C290CE9-14EA-4DF4-9360-C084CCC50C1B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C290CE9-14EA-4DF4-9360-C084CCC50C1B}" name="Tabelle1" displayName="Tabelle1" ref="A1:T74" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" totalsRowBorderDxfId="20">
+  <autoFilter ref="A1:T74" xr:uid="{2C290CE9-14EA-4DF4-9360-C084CCC50C1B}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{E9EA00CB-767A-4E0F-9046-D9C305AB9BE1}" name="Title" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{4944576F-D53E-412A-A718-8D15CEAC1F87}" name="DT Definition" dataDxfId="18"/>
@@ -2105,11 +2096,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC3CDE2-2548-49E4-A153-B9B62C0D483B}">
-  <dimension ref="A1:T79"/>
+  <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N68" sqref="N68"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,3102 +2128,3125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="3" t="s">
+      <c r="S2" s="1"/>
+      <c r="T2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="3"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2" t="s">
+      <c r="O4" s="1"/>
+      <c r="P4" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2" t="s">
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="3" t="s">
+      <c r="S4" s="1"/>
+      <c r="T4" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2" t="s">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="3" t="s">
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2" t="s">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="3" t="s">
+      <c r="S6" s="1"/>
+      <c r="T6" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="3"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2" t="s">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="3"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2" t="s">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S9" s="2"/>
-      <c r="T9" s="3" t="s">
+      <c r="S9" s="1"/>
+      <c r="T9" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="2" t="s">
+      <c r="J10" s="1"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="3"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="3"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="2"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="1"/>
       <c r="H12" t="s">
         <v>313</v>
       </c>
       <c r="I12" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2" t="s">
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S12" s="2"/>
-      <c r="T12" s="3"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="5"/>
       <c r="H13" t="s">
         <v>314</v>
       </c>
       <c r="I13" t="s">
         <v>315</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8" t="s">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="10" t="s">
+      <c r="N13" s="5"/>
+      <c r="O13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="12"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="8" t="s">
+      <c r="D14" s="1"/>
+      <c r="E14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8" t="s">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N14" s="8" t="s">
+      <c r="N14" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="O14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P14" s="8" t="s">
+      <c r="P14" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8" t="s">
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="S14" s="8"/>
-      <c r="T14" s="12"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="9"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8" t="s">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8" t="s">
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8" t="s">
+      <c r="N15" s="5"/>
+      <c r="O15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="12"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="N16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="O16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P16" s="8" t="s">
+      <c r="P16" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8" t="s">
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="S16" s="8" t="s">
+      <c r="S16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="T16" s="12" t="s">
+      <c r="T16" s="9" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8" t="s">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8" t="s">
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="12"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="9"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8" t="s">
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8" t="s">
+      <c r="J18" s="5"/>
+      <c r="K18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M18" s="8" t="s">
+      <c r="M18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="O18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8" t="s">
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S18" s="8"/>
-      <c r="T18" s="12"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="9"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8" t="s">
+      <c r="G19" s="5"/>
+      <c r="H19" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8" t="s">
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="12"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="9"/>
     </row>
     <row r="20" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="10" t="s">
+      <c r="D20" s="3"/>
+      <c r="E20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8" t="s">
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8" t="s">
+      <c r="J20" s="5"/>
+      <c r="K20" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M20" s="8" t="s">
+      <c r="M20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N20" s="8" t="s">
+      <c r="N20" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="O20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P20" s="8" t="s">
+      <c r="P20" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8" t="s">
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S20" s="8"/>
-      <c r="T20" s="12" t="s">
+      <c r="S20" s="5"/>
+      <c r="T20" s="9" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="8" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8" t="s">
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8" t="s">
+      <c r="J21" s="5"/>
+      <c r="K21" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="L21" s="8" t="s">
+      <c r="L21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M21" s="8" t="s">
+      <c r="M21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N21" s="8" t="s">
+      <c r="N21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P21" s="8" t="s">
+      <c r="P21" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8" t="s">
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S21" s="8" t="s">
+      <c r="S21" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="T21" s="12" t="s">
+      <c r="T21" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="12"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="9"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="12"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="9"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="K24" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="M24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="N24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O24" s="8" t="s">
+      <c r="O24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P24" s="8" t="s">
+      <c r="P24" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="Q24" s="8" t="s">
+      <c r="Q24" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="R24" s="8" t="s">
+      <c r="R24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="S24" s="8"/>
-      <c r="T24" s="12" t="s">
+      <c r="S24" s="5"/>
+      <c r="T24" s="9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="1"/>
+      <c r="E25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8" t="s">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8" t="s">
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="12"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="9"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8" t="s">
+      <c r="G26" s="5"/>
+      <c r="H26" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8" t="s">
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="12"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="9"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8" t="s">
+      <c r="G27" s="5"/>
+      <c r="H27" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8" t="s">
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="12"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="8" t="s">
+      <c r="D28" s="1"/>
+      <c r="E28" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8" t="s">
+      <c r="G28" s="5"/>
+      <c r="H28" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8" t="s">
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="12"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="9"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="8" t="s">
+      <c r="D29" s="1"/>
+      <c r="E29" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8" t="s">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8" t="s">
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="12"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="9"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="8" t="s">
+      <c r="D30" s="1"/>
+      <c r="E30" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8" t="s">
+      <c r="G30" s="5"/>
+      <c r="H30" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8" t="s">
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="12"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="9"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="8" t="s">
+      <c r="D31" s="1"/>
+      <c r="E31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8" t="s">
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="I31" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="J31" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8" t="s">
+      <c r="K31" s="5"/>
+      <c r="L31" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="M31" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="N31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O31" s="8" t="s">
+      <c r="O31" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P31" s="8" t="s">
+      <c r="P31" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8" t="s">
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S31" s="8"/>
-      <c r="T31" s="12" t="s">
+      <c r="S31" s="5"/>
+      <c r="T31" s="9" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="8" t="s">
+      <c r="D32" s="1"/>
+      <c r="E32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8" t="s">
+      <c r="G32" s="5"/>
+      <c r="H32" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8" t="s">
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="12"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="9"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="8" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8" t="s">
+      <c r="G33" s="5"/>
+      <c r="H33" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8" t="s">
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="12"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="9"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="8" t="s">
+      <c r="D34" s="1"/>
+      <c r="E34" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8" t="s">
+      <c r="G34" s="5"/>
+      <c r="H34" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8" t="s">
+      <c r="J34" s="5"/>
+      <c r="K34" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8" t="s">
+      <c r="L34" s="5"/>
+      <c r="M34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8" t="s">
+      <c r="N34" s="5"/>
+      <c r="O34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8" t="s">
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="R34" s="8" t="s">
+      <c r="R34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S34" s="8" t="s">
+      <c r="S34" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="T34" s="12"/>
+      <c r="T34" s="9"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8" t="s">
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J35" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8" t="s">
+      <c r="K35" s="5"/>
+      <c r="L35" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M35" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N35" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8" t="s">
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S35" s="8"/>
-      <c r="T35" s="12"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="9"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="12"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="9"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I37" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8" t="s">
+      <c r="J37" s="5"/>
+      <c r="K37" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="L37" s="8" t="s">
+      <c r="L37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M37" s="8" t="s">
+      <c r="M37" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="N37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O37" s="8" t="s">
+      <c r="O37" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8" t="s">
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S37" s="8"/>
-      <c r="T37" s="12"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="9"/>
     </row>
     <row r="38" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="8" t="s">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="I38" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8" t="s">
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="12"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="9"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="8" t="s">
+      <c r="D39" s="1"/>
+      <c r="E39" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8" t="s">
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8" t="s">
+      <c r="J39" s="5"/>
+      <c r="K39" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="L39" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="M39" s="10" t="s">
+      <c r="M39" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="N39" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O39" s="8" t="s">
+      <c r="O39" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8" t="s">
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S39" s="8"/>
-      <c r="T39" s="12" t="s">
+      <c r="S39" s="5"/>
+      <c r="T39" s="9" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8" t="s">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="8" t="s">
+      <c r="D40" s="1"/>
+      <c r="E40" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8" t="s">
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="I40" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="10" t="s">
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="12"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="9"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="12"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="9"/>
     </row>
     <row r="42" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="s">
+      <c r="D42" s="1"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8" t="s">
+      <c r="G42" s="5"/>
+      <c r="H42" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="I42" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8" t="s">
+      <c r="J42" s="5"/>
+      <c r="K42" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="L42" s="8" t="s">
+      <c r="L42" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M42" s="8" t="s">
+      <c r="M42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N42" s="8" t="s">
+      <c r="N42" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O42" s="8" t="s">
+      <c r="O42" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8" t="s">
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="S42" s="8"/>
-      <c r="T42" s="12" t="s">
+      <c r="S42" s="5"/>
+      <c r="T42" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="12"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="9"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="8" t="s">
+      <c r="D44" s="1"/>
+      <c r="E44" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8" t="s">
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J44" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="K44" s="8" t="s">
+      <c r="K44" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="L44" s="8" t="s">
+      <c r="L44" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M44" s="8" t="s">
+      <c r="M44" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="N44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O44" s="8" t="s">
+      <c r="O44" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P44" s="8" t="s">
+      <c r="P44" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8" t="s">
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S44" s="8"/>
-      <c r="T44" s="12"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="9"/>
     </row>
     <row r="45" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8" t="s">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="8" t="s">
+      <c r="D45" s="1"/>
+      <c r="E45" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8" t="s">
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="I45" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8" t="s">
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8" t="s">
+      <c r="N45" s="5"/>
+      <c r="O45" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="12"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="9"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8" t="s">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="8" t="s">
+      <c r="D46" s="1"/>
+      <c r="E46" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8" t="s">
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8" t="s">
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8" t="s">
+      <c r="N46" s="5"/>
+      <c r="O46" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="8"/>
-      <c r="S46" s="8"/>
-      <c r="T46" s="12"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="9"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8" t="s">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="8" t="s">
+      <c r="D47" s="1"/>
+      <c r="E47" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8" t="s">
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8" t="s">
+      <c r="N47" s="5"/>
+      <c r="O47" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="T47" s="12"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="9"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8" t="s">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="8" t="s">
+      <c r="D48" s="1"/>
+      <c r="E48" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8" t="s">
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I48" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8" t="s">
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8" t="s">
+      <c r="N48" s="5"/>
+      <c r="O48" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="8"/>
-      <c r="T48" s="12"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="9"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8" t="s">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8" t="s">
+      <c r="D49" s="1"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="H49" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8" t="s">
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8" t="s">
+      <c r="N49" s="5"/>
+      <c r="O49" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="8"/>
-      <c r="T49" s="12"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="9"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="8" t="s">
+      <c r="D50" s="1"/>
+      <c r="E50" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8" t="s">
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="I50" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8" t="s">
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="M50" s="8" t="s">
+      <c r="M50" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8" t="s">
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="Q50" s="8" t="s">
+      <c r="Q50" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="R50" s="8" t="s">
+      <c r="R50" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S50" s="8"/>
-      <c r="T50" s="12" t="str">
+      <c r="S50" s="5"/>
+      <c r="T50" s="9" t="str">
         <f>LOWER("AUTOMATIC FIRE EXTINGUISHING SYSTEM")</f>
         <v>automatic fire extinguishing system</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8" t="s">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="8" t="s">
+      <c r="D51" s="1"/>
+      <c r="E51" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8" t="s">
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="I51" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8" t="s">
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N51" s="2" t="s">
+      <c r="N51" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O51" s="8" t="s">
+      <c r="O51" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
-      <c r="R51" s="8"/>
-      <c r="S51" s="8"/>
-      <c r="T51" s="12"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="9"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8" t="s">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="8" t="s">
+      <c r="D52" s="1"/>
+      <c r="E52" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8" t="s">
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="I52" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8" t="s">
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N52" s="8"/>
-      <c r="O52" s="8" t="s">
+      <c r="N52" s="5"/>
+      <c r="O52" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P52" s="8"/>
-      <c r="Q52" s="8"/>
-      <c r="R52" s="8"/>
-      <c r="S52" s="8"/>
-      <c r="T52" s="12"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="9"/>
     </row>
     <row r="53" spans="1:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8" t="s">
+      <c r="B53" s="5"/>
+      <c r="C53" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="8" t="s">
+      <c r="D53" s="1"/>
+      <c r="E53" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8" t="s">
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="I53" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8" t="s">
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N53" s="8"/>
-      <c r="O53" s="8" t="s">
+      <c r="N53" s="5"/>
+      <c r="O53" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P53" s="8"/>
-      <c r="Q53" s="8"/>
-      <c r="R53" s="8"/>
-      <c r="S53" s="8"/>
-      <c r="T53" s="12"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="9"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8" t="s">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="8" t="s">
+      <c r="D54" s="1"/>
+      <c r="E54" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8" t="s">
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="I54" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8" t="s">
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N54" s="8"/>
-      <c r="O54" s="8" t="s">
+      <c r="N54" s="5"/>
+      <c r="O54" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P54" s="8"/>
-      <c r="Q54" s="8"/>
-      <c r="R54" s="8"/>
-      <c r="S54" s="8"/>
-      <c r="T54" s="12"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="9"/>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="8" t="s">
+      <c r="D55" s="1"/>
+      <c r="E55" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8" t="s">
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="I55" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8" t="s">
+      <c r="J55" s="5"/>
+      <c r="K55" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="L55" s="8" t="s">
+      <c r="L55" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M55" s="8" t="s">
+      <c r="M55" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="N55" s="8" t="s">
+      <c r="N55" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O55" s="8" t="s">
+      <c r="O55" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P55" s="8"/>
-      <c r="Q55" s="8" t="s">
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="R55" s="8" t="s">
+      <c r="R55" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S55" s="8"/>
-      <c r="T55" s="12" t="s">
+      <c r="S55" s="5"/>
+      <c r="T55" s="9" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8" t="s">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="8"/>
-      <c r="Q56" s="8"/>
-      <c r="R56" s="8"/>
-      <c r="S56" s="8"/>
-      <c r="T56" s="12"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="9"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8" t="s">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8" t="s">
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="I57" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8" t="s">
+      <c r="J57" s="5"/>
+      <c r="K57" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8" t="s">
+      <c r="L57" s="5"/>
+      <c r="M57" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N57" s="2" t="s">
+      <c r="N57" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O57" s="8" t="s">
+      <c r="O57" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P57" s="8"/>
-      <c r="Q57" s="8"/>
-      <c r="R57" s="8" t="s">
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S57" s="8" t="s">
+      <c r="S57" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="T57" s="12"/>
+      <c r="T57" s="9"/>
     </row>
     <row r="58" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="8" t="s">
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8" t="s">
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="I58" s="8" t="s">
+      <c r="I58" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8" t="s">
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N58" s="8"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="8"/>
-      <c r="Q58" s="8"/>
-      <c r="R58" s="8"/>
-      <c r="S58" s="8"/>
-      <c r="T58" s="12"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+      <c r="T58" s="9"/>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="8" t="s">
+      <c r="D59" s="1"/>
+      <c r="E59" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F59" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8" t="s">
+      <c r="G59" s="5"/>
+      <c r="H59" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I59" s="8" t="s">
+      <c r="I59" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8" t="s">
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M59" s="8" t="s">
+      <c r="M59" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N59" s="2" t="s">
+      <c r="N59" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O59" s="8" t="s">
+      <c r="O59" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P59" s="8"/>
-      <c r="Q59" s="8"/>
-      <c r="R59" s="8" t="s">
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S59" s="8"/>
-      <c r="T59" s="12" t="s">
+      <c r="S59" s="5"/>
+      <c r="T59" s="9" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="8" t="s">
+      <c r="D60" s="1"/>
+      <c r="E60" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8" t="s">
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="I60" s="8" t="s">
+      <c r="I60" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8" t="s">
+      <c r="J60" s="5"/>
+      <c r="K60" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="L60" s="8" t="s">
+      <c r="L60" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M60" s="8" t="s">
+      <c r="M60" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N60" s="8"/>
-      <c r="O60" s="8" t="s">
+      <c r="N60" s="5"/>
+      <c r="O60" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P60" s="8"/>
-      <c r="Q60" s="8"/>
-      <c r="R60" s="8" t="s">
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S60" s="8"/>
-      <c r="T60" s="12" t="s">
+      <c r="S60" s="5"/>
+      <c r="T60" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8" t="s">
+      <c r="B61" s="5"/>
+      <c r="C61" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="8" t="s">
+      <c r="D61" s="1"/>
+      <c r="E61" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8" t="s">
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="I61" s="8" t="s">
+      <c r="I61" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="8"/>
-      <c r="M61" s="8" t="s">
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N61" s="8"/>
-      <c r="O61" s="8"/>
-      <c r="P61" s="8"/>
-      <c r="Q61" s="8"/>
-      <c r="R61" s="8"/>
-      <c r="S61" s="8"/>
-      <c r="T61" s="12"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="9"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8" t="s">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D62" s="2"/>
-      <c r="E62" s="8" t="s">
+      <c r="D62" s="1"/>
+      <c r="E62" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8" t="s">
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="I62" s="8" t="s">
+      <c r="I62" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
-      <c r="M62" s="8" t="s">
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N62" s="8"/>
-      <c r="O62" s="8"/>
-      <c r="P62" s="8"/>
-      <c r="Q62" s="8"/>
-      <c r="R62" s="8"/>
-      <c r="S62" s="8"/>
-      <c r="T62" s="12"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+      <c r="T62" s="9"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8" t="s">
+      <c r="B63" s="5"/>
+      <c r="C63" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8" t="s">
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="I63" s="8" t="s">
+      <c r="I63" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
-      <c r="M63" s="8" t="s">
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N63" s="8"/>
-      <c r="O63" s="8"/>
-      <c r="P63" s="8"/>
-      <c r="Q63" s="8"/>
-      <c r="R63" s="8"/>
-      <c r="S63" s="8"/>
-      <c r="T63" s="12"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+      <c r="T63" s="9"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="8" t="s">
+      <c r="D64" s="1"/>
+      <c r="E64" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F64" s="8" t="s">
+      <c r="F64" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8" t="s">
+      <c r="G64" s="5"/>
+      <c r="H64" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I64" s="8" t="s">
+      <c r="I64" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="J64" s="8" t="s">
+      <c r="J64" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="K64" s="8" t="s">
+      <c r="K64" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="L64" s="8" t="s">
+      <c r="L64" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="M64" s="8" t="s">
+      <c r="M64" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N64" s="8" t="s">
+      <c r="N64" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O64" s="8" t="s">
+      <c r="O64" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P64" s="8"/>
-      <c r="Q64" s="8"/>
-      <c r="R64" s="8" t="s">
+      <c r="P64" s="5"/>
+      <c r="Q64" s="5"/>
+      <c r="R64" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S64" s="8"/>
-      <c r="T64" s="12" t="s">
+      <c r="S64" s="5"/>
+      <c r="T64" s="9" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8" t="s">
+      <c r="B65" s="5"/>
+      <c r="C65" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="D65" s="2"/>
-      <c r="E65" s="8" t="s">
+      <c r="D65" s="1"/>
+      <c r="E65" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="8" t="s">
+      <c r="F65" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8" t="s">
+      <c r="G65" s="5"/>
+      <c r="H65" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I65" s="8" t="s">
+      <c r="I65" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="J65" s="8"/>
-      <c r="K65" s="8"/>
-      <c r="L65" s="8"/>
-      <c r="M65" s="8" t="s">
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N65" s="8"/>
-      <c r="O65" s="8"/>
-      <c r="P65" s="8"/>
-      <c r="Q65" s="8"/>
-      <c r="R65" s="8"/>
-      <c r="S65" s="8"/>
-      <c r="T65" s="12"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
+      <c r="P65" s="5"/>
+      <c r="Q65" s="5"/>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5"/>
+      <c r="T65" s="9"/>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8" t="s">
+      <c r="B66" s="5"/>
+      <c r="C66" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="8"/>
-      <c r="O66" s="8"/>
-      <c r="P66" s="8"/>
-      <c r="Q66" s="8"/>
-      <c r="R66" s="8"/>
-      <c r="S66" s="8"/>
-      <c r="T66" s="12"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="5"/>
+      <c r="Q66" s="5"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+      <c r="T66" s="9"/>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="8" t="s">
+      <c r="D67" s="1"/>
+      <c r="E67" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8" t="s">
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="I67" s="8" t="s">
+      <c r="I67" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="J67" s="8"/>
-      <c r="K67" s="8"/>
-      <c r="L67" s="8" t="s">
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M67" s="8" t="s">
+      <c r="M67" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N67" s="2" t="s">
+      <c r="N67" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O67" s="8" t="s">
+      <c r="O67" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P67" s="8" t="s">
+      <c r="P67" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="Q67" s="8"/>
-      <c r="R67" s="8" t="s">
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S67" s="8"/>
-      <c r="T67" s="12"/>
+      <c r="S67" s="5"/>
+      <c r="T67" s="9"/>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8" t="s">
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="8" t="s">
+      <c r="D68" s="1"/>
+      <c r="E68" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8" t="s">
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="I68" s="8" t="s">
+      <c r="I68" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="8"/>
-      <c r="M68" s="8" t="s">
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N68" s="8"/>
-      <c r="O68" s="8"/>
-      <c r="P68" s="8"/>
-      <c r="Q68" s="8"/>
-      <c r="R68" s="8"/>
-      <c r="S68" s="8"/>
-      <c r="T68" s="12"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+      <c r="T68" s="9"/>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8" t="s">
+      <c r="B69" s="5"/>
+      <c r="C69" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="D69" s="2"/>
-      <c r="E69" s="8" t="s">
+      <c r="D69" s="1"/>
+      <c r="E69" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8" t="s">
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="I69" s="8" t="s">
+      <c r="I69" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8"/>
-      <c r="M69" s="8" t="s">
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N69" s="8"/>
-      <c r="O69" s="8"/>
-      <c r="P69" s="8"/>
-      <c r="Q69" s="8"/>
-      <c r="R69" s="8"/>
-      <c r="S69" s="8"/>
-      <c r="T69" s="12"/>
+      <c r="N69" s="5"/>
+      <c r="O69" s="5"/>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="5"/>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="9"/>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
+      <c r="A70" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E70" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8" t="s">
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="I70" s="8" t="s">
+      <c r="I70" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8" t="s">
+      <c r="J70" s="5"/>
+      <c r="K70" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="L70" s="8" t="s">
+      <c r="L70" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="M70" s="8" t="s">
+      <c r="M70" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N70" s="2" t="s">
+      <c r="N70" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O70" s="8" t="s">
+      <c r="O70" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="P70" s="8"/>
-      <c r="Q70" s="8"/>
-      <c r="R70" s="8" t="s">
+      <c r="P70" s="5"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S70" s="8"/>
-      <c r="T70" s="12"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="9"/>
     </row>
     <row r="71" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E71" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8" t="s">
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="I71" s="8" t="s">
+      <c r="I71" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8" t="s">
+      <c r="J71" s="5"/>
+      <c r="K71" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="L71" s="8" t="s">
+      <c r="L71" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M71" s="8" t="s">
+      <c r="M71" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N71" s="2" t="s">
+      <c r="N71" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O71" s="8" t="s">
+      <c r="O71" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P71" s="8"/>
-      <c r="Q71" s="8"/>
-      <c r="R71" s="8" t="s">
+      <c r="P71" s="5"/>
+      <c r="Q71" s="5"/>
+      <c r="R71" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S71" s="8"/>
-      <c r="T71" s="12"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="9"/>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="18" t="s">
+      <c r="A72" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="8" t="s">
+      <c r="D72" s="1"/>
+      <c r="E72" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F72" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8" t="s">
+      <c r="G72" s="5"/>
+      <c r="H72" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="I72" s="8" t="s">
+      <c r="I72" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="J72" s="8" t="s">
+      <c r="J72" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="K72" s="8" t="s">
+      <c r="K72" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="L72" s="8" t="s">
+      <c r="L72" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="M72" s="8" t="s">
+      <c r="M72" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N72" s="2" t="s">
+      <c r="N72" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O72" s="8" t="s">
+      <c r="O72" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P72" s="8"/>
-      <c r="Q72" s="8"/>
-      <c r="R72" s="8" t="s">
+      <c r="P72" s="5"/>
+      <c r="Q72" s="5"/>
+      <c r="R72" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S72" s="8"/>
-      <c r="T72" s="12" t="s">
+      <c r="S72" s="5"/>
+      <c r="T72" s="9" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="8" t="s">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F73" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8" t="s">
+      <c r="G73" s="5"/>
+      <c r="H73" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="I73" s="8" t="s">
+      <c r="I73" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="J73" s="8"/>
-      <c r="K73" s="8"/>
-      <c r="L73" s="8"/>
-      <c r="M73" s="8" t="s">
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N73" s="8"/>
-      <c r="O73" s="8"/>
-      <c r="P73" s="8"/>
-      <c r="Q73" s="8"/>
-      <c r="R73" s="8"/>
-      <c r="S73" s="8"/>
-      <c r="T73" s="12"/>
+      <c r="N73" s="5"/>
+      <c r="O73" s="5"/>
+      <c r="P73" s="5"/>
+      <c r="Q73" s="5"/>
+      <c r="R73" s="5"/>
+      <c r="S73" s="5"/>
+      <c r="T73" s="9"/>
     </row>
     <row r="74" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="8" t="s">
+      <c r="D74" s="4"/>
+      <c r="E74" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F74" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8" t="s">
+      <c r="G74" s="6"/>
+      <c r="H74" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="I74" s="8" t="s">
+      <c r="I74" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="J74" s="8" t="s">
+      <c r="J74" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="K74" s="8" t="s">
+      <c r="K74" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="L74" s="8" t="s">
+      <c r="L74" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M74" s="8" t="s">
+      <c r="M74" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="N74" s="8"/>
-      <c r="O74" s="8" t="s">
+      <c r="N74" s="6"/>
+      <c r="O74" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P74" s="8"/>
-      <c r="Q74" s="8"/>
-      <c r="R74" s="8" t="s">
+      <c r="P74" s="6"/>
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="S74" s="8"/>
-      <c r="T74" s="12" t="s">
+      <c r="S74" s="6"/>
+      <c r="T74" s="10" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="75" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="8"/>
-      <c r="L75" s="8"/>
-      <c r="M75" s="8"/>
-      <c r="N75" s="8"/>
-      <c r="O75" s="8"/>
-      <c r="P75" s="8"/>
-      <c r="Q75" s="8"/>
-      <c r="R75" s="8"/>
-      <c r="S75" s="8"/>
-      <c r="T75" s="12"/>
+      <c r="A75" s="18"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="18"/>
+      <c r="M75" s="18"/>
+      <c r="N75" s="18"/>
+      <c r="O75" s="18"/>
+      <c r="P75" s="18"/>
+      <c r="Q75" s="18"/>
+      <c r="R75" s="18"/>
+      <c r="S75" s="18"/>
+      <c r="T75" s="18"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
-      <c r="J76" s="8"/>
-      <c r="K76" s="8"/>
-      <c r="L76" s="8"/>
-      <c r="M76" s="8"/>
-      <c r="N76" s="8"/>
-      <c r="O76" s="8"/>
-      <c r="P76" s="8"/>
-      <c r="Q76" s="8"/>
-      <c r="R76" s="8"/>
-      <c r="S76" s="8"/>
-      <c r="T76" s="12"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="18"/>
+      <c r="M76" s="18"/>
+      <c r="N76" s="18"/>
+      <c r="O76" s="18"/>
+      <c r="P76" s="18"/>
+      <c r="Q76" s="18"/>
+      <c r="R76" s="18"/>
+      <c r="S76" s="18"/>
+      <c r="T76" s="18"/>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
-      <c r="J77" s="8"/>
-      <c r="K77" s="8"/>
-      <c r="L77" s="8"/>
-      <c r="M77" s="8"/>
-      <c r="N77" s="8"/>
-      <c r="O77" s="8"/>
-      <c r="P77" s="8"/>
-      <c r="Q77" s="8"/>
-      <c r="R77" s="8"/>
-      <c r="S77" s="8"/>
-      <c r="T77" s="12"/>
+      <c r="A77" s="18"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18"/>
+      <c r="L77" s="18"/>
+      <c r="M77" s="18"/>
+      <c r="N77" s="18"/>
+      <c r="O77" s="18"/>
+      <c r="P77" s="18"/>
+      <c r="Q77" s="18"/>
+      <c r="R77" s="18"/>
+      <c r="S77" s="18"/>
+      <c r="T77" s="18"/>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A78" s="7"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="9"/>
-      <c r="L78" s="9"/>
-      <c r="M78" s="9"/>
-      <c r="N78" s="9"/>
-      <c r="O78" s="9"/>
-      <c r="P78" s="9"/>
-      <c r="Q78" s="9"/>
-      <c r="R78" s="9"/>
-      <c r="S78" s="9"/>
-      <c r="T78" s="13"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="18"/>
+      <c r="P78" s="18"/>
+      <c r="Q78" s="18"/>
+      <c r="R78" s="18"/>
+      <c r="S78" s="18"/>
+      <c r="T78" s="18"/>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
-      <c r="N79" s="1"/>
-      <c r="O79" s="1"/>
-      <c r="P79" s="1"/>
-      <c r="Q79" s="1"/>
-      <c r="R79" s="1"/>
-      <c r="S79" s="1"/>
+      <c r="A79" s="19"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+      <c r="K79" s="19"/>
+      <c r="L79" s="19"/>
+      <c r="M79" s="19"/>
+      <c r="N79" s="19"/>
+      <c r="O79" s="19"/>
+      <c r="P79" s="19"/>
+      <c r="Q79" s="19"/>
+      <c r="R79" s="19"/>
+      <c r="S79" s="19"/>
+      <c r="T79" s="19"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A80" s="19"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
+      <c r="L80" s="19"/>
+      <c r="M80" s="19"/>
+      <c r="N80" s="19"/>
+      <c r="O80" s="19"/>
+      <c r="P80" s="19"/>
+      <c r="Q80" s="19"/>
+      <c r="R80" s="19"/>
+      <c r="S80" s="19"/>
+      <c r="T80" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update visualizations in cleanup file
</commit_message>
<xml_diff>
--- a/extraction consolidation results_V0_1.xlsx
+++ b/extraction consolidation results_V0_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac130903\Desktop\MDE4DT\mde4dts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E7A9595-4895-4044-8CE0-85B0DBDBBF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4A0F0338-BB40-4B25-8F67-33B08D86E8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D11C759-8767-4256-9E25-90A34587B317}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="327">
   <si>
     <t>Title</t>
   </si>
@@ -1018,13 +1018,16 @@
   </si>
   <si>
     <t>Fault Tree</t>
+  </si>
+  <si>
+    <t>SysML: BDD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1073,8 +1076,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1101,8 +1112,13 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1229,15 +1245,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1258,13 +1290,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="5" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -2098,9 +2133,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC3CDE2-2548-49E4-A153-B9B62C0D483B}">
   <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F37" sqref="F37:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,10 +2169,10 @@
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="21" t="s">
         <v>278</v>
       </c>
       <c r="E1" s="12" t="s">
@@ -2155,7 +2190,7 @@
       <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="20" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="11" t="s">
@@ -2197,7 +2232,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>284</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -2208,7 +2243,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>326</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>23</v>
@@ -2493,7 +2528,9 @@
       <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
         <v>58</v>
@@ -2543,7 +2580,9 @@
       <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
         <v>59</v>

</xml_diff>